<commit_message>
Create Adapter View "Begin View"
Create an adapter view to seperate different rollers
</commit_message>
<xml_diff>
--- a/Document/Work Protocol.xlsx
+++ b/Document/Work Protocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
   <si>
     <t>Module</t>
   </si>
@@ -25,9 +25,6 @@
   </si>
   <si>
     <t>Plan</t>
-  </si>
-  <si>
-    <t>View I</t>
   </si>
   <si>
     <t>Communication</t>
@@ -98,6 +95,54 @@
   <si>
     <t>[9/28/2014]
 Create UserData.</t>
+  </si>
+  <si>
+    <t>Login View</t>
+  </si>
+  <si>
+    <t>Sub Module</t>
+  </si>
+  <si>
+    <t>View</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Controler</t>
+  </si>
+  <si>
+    <t>Begin View</t>
+  </si>
+  <si>
+    <t>[9/30/2014]
+Create an adpter view to combinate the Slave and Master modes.
+-Press "I'm coming" to go to the slave mode;
+-Press "I'm waiting" to go to the master mode.</t>
+  </si>
+  <si>
+    <t>Should be change its name to Master View</t>
+  </si>
+  <si>
+    <t>Used in Master roller, can check the position of others</t>
+  </si>
+  <si>
+    <t>Let user to select ist roller: slave or master</t>
+  </si>
+  <si>
+    <t>Master View</t>
+  </si>
+  <si>
+    <t>Slave View</t>
+  </si>
+  <si>
+    <t>Used in Slave roller</t>
+  </si>
+  <si>
+    <t>System Archtecture</t>
+  </si>
+  <si>
+    <t>Shall we seperate the two roller between Slave and Master?</t>
   </si>
 </sst>
 </file>
@@ -132,7 +177,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -149,8 +194,13 @@
         <fgColor theme="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -173,13 +223,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
@@ -200,8 +288,20 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Accent3" xfId="3" builtinId="37"/>
     <cellStyle name="Accent6" xfId="2" builtinId="49"/>
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,121 +615,212 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
     <col min="2" max="2" width="21.140625" customWidth="1"/>
     <col min="3" max="3" width="41.28515625" customWidth="1"/>
     <col min="4" max="4" width="36.140625" customWidth="1"/>
+    <col min="5" max="5" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="12"/>
+      <c r="B3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="12"/>
+      <c r="B4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="11"/>
+      <c r="B5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="B17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+    </row>
+    <row r="19" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+    </row>
+    <row r="21" spans="1:4" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:4" ht="135" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:4" ht="120" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-    </row>
-    <row r="12" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C15" s="3"/>
-    </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>23</v>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+    </row>
+    <row r="25" spans="1:4" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -653,35 +844,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>14</v>
-      </c>
-      <c r="C1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="9">
         <v>41910</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="9">
         <v>41910</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>